<commit_message>
initial 2023/24 season commit
</commit_message>
<xml_diff>
--- a/inputs/manager_ids.xlsx
+++ b/inputs/manager_ids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\MIDept\3_All Staff Folders\Clinical Outcomes Analysis Team\02 Projects\04 R Projects\fantasy_premier_league\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94BE214-629E-4A26-ACA7-7ACDE20FC664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616CC1CB-FB3F-45DB-B3D8-32BF4EE99BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{B56F89CB-8CD1-4225-B498-8B1B9FA841E5}"/>
+    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{B56F89CB-8CD1-4225-B498-8B1B9FA841E5}"/>
   </bookViews>
   <sheets>
     <sheet name="manager_ids" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
   <si>
     <t>id</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Season 22-23</t>
+  </si>
+  <si>
+    <t>Season 23-24</t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66772506-0846-4296-B70F-9AB992D811DA}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -848,6 +851,34 @@
         <v>38533</v>
       </c>
     </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>2564951</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="2">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>2565192</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="2">
+        <v>12345</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D28">
     <sortCondition ref="C2:C28"/>

</xml_diff>

<commit_message>
start of season update
</commit_message>
<xml_diff>
--- a/inputs/manager_ids.xlsx
+++ b/inputs/manager_ids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\3_All Staff Folders\Clinical Outcomes Analysis Team\02 Projects\04 R Projects\fantasy_premier_league\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9E59DE-B3AA-46F7-BC87-160CC1114C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4557E22F-129A-42DE-B36F-7F0F076DDC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{B56F89CB-8CD1-4225-B498-8B1B9FA841E5}"/>
+    <workbookView xWindow="120" yWindow="570" windowWidth="28305" windowHeight="15270" xr2:uid="{B56F89CB-8CD1-4225-B498-8B1B9FA841E5}"/>
   </bookViews>
   <sheets>
     <sheet name="manager_ids" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>Season 24-25</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -475,7 +472,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -489,7 +486,7 @@
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>1234</v>
       </c>
     </row>
@@ -503,7 +500,7 @@
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>1234</v>
       </c>
     </row>
@@ -517,7 +514,7 @@
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>1234</v>
       </c>
     </row>
@@ -531,7 +528,7 @@
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>1234</v>
       </c>
     </row>
@@ -545,7 +542,7 @@
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>1234</v>
       </c>
     </row>
@@ -559,7 +556,7 @@
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>1234</v>
       </c>
     </row>
@@ -573,7 +570,7 @@
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>1234</v>
       </c>
     </row>
@@ -587,7 +584,7 @@
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>1234</v>
       </c>
     </row>
@@ -601,7 +598,7 @@
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>1234</v>
       </c>
     </row>
@@ -615,7 +612,7 @@
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>3550</v>
       </c>
     </row>
@@ -629,7 +626,7 @@
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>3550</v>
       </c>
     </row>
@@ -643,7 +640,7 @@
       <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>3550</v>
       </c>
     </row>
@@ -657,7 +654,7 @@
       <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>3550</v>
       </c>
     </row>
@@ -671,7 +668,7 @@
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>3550</v>
       </c>
     </row>
@@ -685,7 +682,7 @@
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>3550</v>
       </c>
     </row>
@@ -699,7 +696,7 @@
       <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>3550</v>
       </c>
     </row>
@@ -713,7 +710,7 @@
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>3550</v>
       </c>
     </row>
@@ -727,7 +724,7 @@
       <c r="C19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>3550</v>
       </c>
     </row>
@@ -741,7 +738,7 @@
       <c r="C20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>38533</v>
       </c>
     </row>
@@ -755,7 +752,7 @@
       <c r="C21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>38533</v>
       </c>
     </row>
@@ -769,7 +766,7 @@
       <c r="C22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>38533</v>
       </c>
     </row>
@@ -783,7 +780,7 @@
       <c r="C23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>38533</v>
       </c>
     </row>
@@ -797,7 +794,7 @@
       <c r="C24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>38533</v>
       </c>
     </row>
@@ -811,7 +808,7 @@
       <c r="C25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>38533</v>
       </c>
     </row>
@@ -825,7 +822,7 @@
       <c r="C26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="1">
         <v>38533</v>
       </c>
     </row>
@@ -839,7 +836,7 @@
       <c r="C27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <v>38533</v>
       </c>
     </row>
@@ -853,7 +850,7 @@
       <c r="C28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>38533</v>
       </c>
     </row>
@@ -867,7 +864,7 @@
       <c r="C29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <v>149616</v>
       </c>
     </row>
@@ -881,7 +878,7 @@
       <c r="C30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="1">
         <v>149616</v>
       </c>
     </row>
@@ -895,7 +892,7 @@
       <c r="C31" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="1">
         <v>149616</v>
       </c>
     </row>
@@ -909,7 +906,7 @@
       <c r="C32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="1">
         <v>149616</v>
       </c>
     </row>
@@ -923,7 +920,7 @@
       <c r="C33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="1">
         <v>149616</v>
       </c>
     </row>
@@ -937,7 +934,7 @@
       <c r="C34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="1">
         <v>149616</v>
       </c>
     </row>
@@ -951,7 +948,7 @@
       <c r="C35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="1">
         <v>149616</v>
       </c>
     </row>
@@ -965,7 +962,7 @@
       <c r="C36" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="1">
         <v>149616</v>
       </c>
     </row>
@@ -979,7 +976,7 @@
       <c r="C37" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="1">
         <v>149616</v>
       </c>
     </row>
@@ -993,8 +990,8 @@
       <c r="C38" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>18</v>
+      <c r="D38" s="1">
+        <v>20232</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1007,85 +1004,106 @@
       <c r="C39" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>18</v>
+      <c r="D39" s="1">
+        <v>20232</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>1114016</v>
+      </c>
       <c r="B40" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>18</v>
+      <c r="D40" s="1">
+        <v>20232</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>109884</v>
+      </c>
       <c r="B41" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>18</v>
+      <c r="D41" s="1">
+        <v>20232</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>6188948</v>
+      </c>
       <c r="B42" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>18</v>
+      <c r="D42" s="1">
+        <v>20232</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>1123161</v>
+      </c>
       <c r="B43" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>18</v>
+      <c r="D43" s="1">
+        <v>20232</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>10946</v>
+      </c>
       <c r="B44" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>18</v>
+      <c r="D44" s="1">
+        <v>20232</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>6186573</v>
+      </c>
       <c r="B45" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>18</v>
+      <c r="D45" s="1">
+        <v>20232</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>1077612</v>
+      </c>
       <c r="B46" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>18</v>
+      <c r="D46" s="1">
+        <v>20232</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>